<commit_message>
create and delete admin actions added
</commit_message>
<xml_diff>
--- a/scrum/burndown_template.xlsx
+++ b/scrum/burndown_template.xlsx
@@ -1,37 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://msudenver-my.sharepoint.com/personal/tmota_msudenver_edu/Documents/Teaching/Courses/__24SCS3250_SE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarah\OneDrive\Desktop\School\2024\Fall\SWDevCS-3250-002\CS3250\Program3\prog3thedreamteam\scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7397B228-E7AA-634C-96A5-F3624B942EAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AC498A-B4A1-489F-8226-70D8C02BB416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15020" xr2:uid="{7A4C5A10-B1D5-9946-8D6C-7E3C0798020F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7A4C5A10-B1D5-9946-8D6C-7E3C0798020F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$C$1:$G$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$C$2:$G$2</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$C$3:$G$3</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$C$1:$G$1</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$C$2:$G$2</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$C$3:$G$3</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$C$3:$G$3</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$C$4:$G$4</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$C$1:$G$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$C$2:$G$2</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$C$3:$G$3</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$C$4:$G$4</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$C$1:$G$1</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$C$2:$G$2</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -52,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -61,12 +45,6 @@
   </si>
   <si>
     <t>Sprint 3</t>
-  </si>
-  <si>
-    <t>Sprint 4</t>
-  </si>
-  <si>
-    <t>Sprint 5</t>
   </si>
   <si>
     <t>Planned</t>
@@ -83,12 +61,21 @@
   <si>
     <t>Ideal</t>
   </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -100,6 +87,14 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -158,9 +153,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -170,6 +165,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -288,9 +286,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$1:$G$1</c:f>
+              <c:f>Sheet1!$C$1:$E$1</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Sprint 1</c:v>
                 </c:pt>
@@ -300,35 +298,23 @@
                 <c:pt idx="2">
                   <c:v>Sprint 3</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>Sprint 4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sprint 5</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$G$2</c:f>
+              <c:f>Sheet1!$C$2:$E$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>75</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>60</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -357,9 +343,9 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$1:$G$1</c:f>
+              <c:f>Sheet1!$C$1:$E$1</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>Sprint 1</c:v>
                 </c:pt>
@@ -369,35 +355,23 @@
                 <c:pt idx="2">
                   <c:v>Sprint 3</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>Sprint 4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Sprint 5</c:v>
-                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$G$3</c:f>
+              <c:f>Sheet1!$C$3:$E$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>65</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -443,24 +417,18 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$4:$G$4</c:f>
+              <c:f>Sheet1!$C$4:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>175</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>140</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -492,24 +460,18 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$5:$G$5</c:f>
+              <c:f>Sheet1!$C$5:$E$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>200</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>155</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1287,13 +1249,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>29936</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>178708</xdr:rowOff>
@@ -1325,9 +1287,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1365,7 +1327,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1471,7 +1433,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1613,7 +1575,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1621,21 +1583,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ADD8F6-D520-684C-80D6-92D618A9A1CC}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.6640625" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="2" width="11.625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -1646,107 +1608,135 @@
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3">
-        <v>75</v>
+        <v>6</v>
       </c>
       <c r="D2" s="3">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="E2" s="3">
-        <v>80</v>
-      </c>
-      <c r="F2" s="3">
-        <v>40</v>
-      </c>
-      <c r="G2" s="3">
-        <v>40</v>
+        <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="D3" s="4">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="E3" s="4">
-        <v>65</v>
-      </c>
-      <c r="F3" s="4">
-        <v>50</v>
-      </c>
-      <c r="G3" s="4">
-        <v>40</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3">
-        <f>B5-C2</f>
-        <v>175</v>
+        <v>16</v>
       </c>
       <c r="D4" s="3">
-        <f t="shared" ref="D4:G4" si="0">C5-D2</f>
-        <v>140</v>
+        <v>23</v>
       </c>
       <c r="E4" s="3">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
-      <c r="F4" s="3">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="G4" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" s="4">
-        <v>250</v>
+        <v>44</v>
       </c>
       <c r="C5" s="4">
-        <f>B5-C3</f>
-        <v>200</v>
+        <f>$B$5-SUM(B3:C3)</f>
+        <v>41</v>
       </c>
       <c r="D5" s="4">
-        <f t="shared" ref="D5:G5" si="1">C5-D3</f>
-        <v>155</v>
+        <f>$B$5-SUM(C3:D3)</f>
+        <v>18</v>
       </c>
       <c r="E5" s="4">
-        <f t="shared" si="1"/>
-        <v>90</v>
-      </c>
-      <c r="F5" s="4">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="G5" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f>$B$5-SUM(C3:D3)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>3</v>
+      </c>
+      <c r="B11" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>6</v>
+      </c>
+      <c r="B14" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="5">
+        <f>SUM(B9:B14)</f>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1, 2, 4,5 complete
</commit_message>
<xml_diff>
--- a/scrum/burndown_template.xlsx
+++ b/scrum/burndown_template.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarah\OneDrive\Desktop\School\2024\Fall\SWDevCS-3250-002\CS3250\Program3\prog3thedreamteam\scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AC498A-B4A1-489F-8226-70D8C02BB416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D7997C-FF27-4CCA-AA66-51D78ADF9C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7A4C5A10-B1D5-9946-8D6C-7E3C0798020F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
+    <sheet name="User Stories" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -69,6 +70,30 @@
   </si>
   <si>
     <t>Total:</t>
+  </si>
+  <si>
+    <t>The website lists all items curently available by store on the homepage with no log in required</t>
+  </si>
+  <si>
+    <t>The restaurant has an Admin account able to add new items and delete old items on the menu through the back end.</t>
+  </si>
+  <si>
+    <t>The restaurant has an Admin account able to update items on the menu through the back end.    </t>
+  </si>
+  <si>
+    <t>Restaurant customers should be able to add and remove items from their purchase cart. The purchase screen will total all added items.</t>
+  </si>
+  <si>
+    <t>Restaurant customers should be able to browse and sort the menu by categories: appetizers, entrees, desserts, beverages, and sides.</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Done?</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -153,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -170,11 +195,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -222,11 +269,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Project's</a:t>
+              <a:t>Mystic</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Title</a:t>
+              <a:t> Menu</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -286,7 +333,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$1:$E$1</c:f>
+              <c:f>'Burndown Chart'!$C$1:$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -303,7 +350,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$E$2</c:f>
+              <c:f>'Burndown Chart'!$C$2:$E$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -343,7 +390,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$1:$E$1</c:f>
+              <c:f>'Burndown Chart'!$C$1:$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -360,7 +407,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$E$3</c:f>
+              <c:f>'Burndown Chart'!$C$3:$E$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -368,7 +415,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>18</c:v>
@@ -417,7 +464,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$4:$E$4</c:f>
+              <c:f>'Burndown Chart'!$C$4:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -460,7 +507,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$5:$E$5</c:f>
+              <c:f>'Burndown Chart'!$C$5:$E$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -468,10 +515,10 @@
                   <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1286,6 +1333,19 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A0EF6A37-4748-4DEC-B7FD-72A82AF328E5}" name="Table1" displayName="Table1" ref="A1:D8" totalsRowShown="0" headerRowDxfId="3" dataDxfId="4">
+  <autoFilter ref="A1:D8" xr:uid="{A0EF6A37-4748-4DEC-B7FD-72A82AF328E5}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{AA7BF314-D841-48CF-A884-BC146FCD5284}" name="US" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{8190B0CE-E294-4B2E-991B-EA9F50E7BDDA}" name="Points" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{83DEA946-CA93-4BA9-A541-CC733B6F02EC}" name="Column1" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{F6DA7E5C-43AB-4498-B504-C1CA4448B18E}" name="Done?" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -1583,10 +1643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46ADD8F6-D520-684C-80D6-92D618A9A1CC}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1633,7 +1693,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="4">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E3" s="4">
         <v>18</v>
@@ -1667,80 +1727,143 @@
       </c>
       <c r="D5" s="4">
         <f>$B$5-SUM(C3:D3)</f>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E5" s="4">
         <f>$B$5-SUM(C3:D3)</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>1</v>
-      </c>
-      <c r="B9" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>2</v>
-      </c>
-      <c r="B10" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>3</v>
-      </c>
-      <c r="B11" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>5</v>
-      </c>
-      <c r="B13" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>6</v>
-      </c>
-      <c r="B14" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="5">
-        <f>SUM(B9:B14)</f>
-        <v>44</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B56DDBE7-1AE2-45E5-9AB4-39447E44C30B}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="98.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>3</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>10</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="G4">
+        <f>SUM(B3,B5,B6)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>10</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>13</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="5">
+        <f>SUM(B2:B7)</f>
+        <v>44</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding 1/2 tests, updated burndown
</commit_message>
<xml_diff>
--- a/scrum/burndown_template.xlsx
+++ b/scrum/burndown_template.xlsx
@@ -8,9 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarah\OneDrive\Desktop\School\2024\Fall\SWDevCS-3250-002\CS3250\Program3\prog3thedreamteam\scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D7997C-FF27-4CCA-AA66-51D78ADF9C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB84CA7E-277F-44E9-AC8D-5594ABAD1873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7A4C5A10-B1D5-9946-8D6C-7E3C0798020F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{95F43B3A-D861-42A2-933E-093E9D903741}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -94,13 +95,19 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>*total not including optional</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -120,6 +127,13 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -178,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -197,6 +211,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -361,7 +378,7 @@
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>118</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -418,7 +435,7 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -512,13 +529,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>41</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1334,10 +1351,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A0EF6A37-4748-4DEC-B7FD-72A82AF328E5}" name="Table1" displayName="Table1" ref="A1:D8" totalsRowShown="0" headerRowDxfId="3" dataDxfId="4">
-  <autoFilter ref="A1:D8" xr:uid="{A0EF6A37-4748-4DEC-B7FD-72A82AF328E5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A0EF6A37-4748-4DEC-B7FD-72A82AF328E5}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D9" xr:uid="{A0EF6A37-4748-4DEC-B7FD-72A82AF328E5}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{AA7BF314-D841-48CF-A884-BC146FCD5284}" name="US" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{AA7BF314-D841-48CF-A884-BC146FCD5284}" name="US" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{8190B0CE-E294-4B2E-991B-EA9F50E7BDDA}" name="Points" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{83DEA946-CA93-4BA9-A541-CC733B6F02EC}" name="Column1" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{F6DA7E5C-43AB-4498-B504-C1CA4448B18E}" name="Done?" dataDxfId="0"/>
@@ -1646,8 +1663,9 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1681,7 +1699,7 @@
         <v>23</v>
       </c>
       <c r="E2" s="3">
-        <v>118</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1696,7 +1714,7 @@
         <v>18</v>
       </c>
       <c r="E3" s="4">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1719,19 +1737,19 @@
         <v>5</v>
       </c>
       <c r="B5" s="4">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C5" s="4">
-        <f>$B$5-SUM(B3:C3)</f>
-        <v>41</v>
+        <f>$B$5-SUM(C3)</f>
+        <v>28</v>
       </c>
       <c r="D5" s="4">
         <f>$B$5-SUM(C3:D3)</f>
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="E5" s="4">
-        <f>$B$5-SUM(C3:D3)</f>
-        <v>23</v>
+        <f>$B$5-SUM(C3:E3)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1742,10 +1760,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B56DDBE7-1AE2-45E5-9AB4-39447E44C30B}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1753,7 +1774,7 @@
     <col min="3" max="3" width="98.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1767,7 +1788,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1780,8 +1801,11 @@
       <c r="D2" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1794,8 +1818,12 @@
       <c r="D3" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="F3">
+        <f>SUM(Table1[[#This Row],[Points]],B5,B6)</f>
+        <v>18</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1805,13 +1833,15 @@
       <c r="C4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="G4">
-        <f>SUM(B3,B5,B6)</f>
+      <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="F4">
+        <f>Table1[[#This Row],[Points]]</f>
+        <v>10</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1824,8 +1854,12 @@
       <c r="D5" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="F5">
+        <f>SUM(F2:F4)</f>
+        <v>31</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1839,26 +1873,36 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>13</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="5">
-        <f>SUM(B2:B7)</f>
-        <v>44</v>
+        <f>SUM(B2:B6)</f>
+        <v>31</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>